<commit_message>
GetThread function needs to be fixed. Not working for .NET 5
</commit_message>
<xml_diff>
--- a/StartHereExample/Examples.xlsx
+++ b/StartHereExample/Examples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkSpace\xlwDotNet-Examples\StartHereExample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0053B6F8-6150-4B67-B49B-32E6C7C1F727}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58231DDF-37FD-4F03-BA6A-C11B0A0C0DA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataFromYahoo" sheetId="3" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <definedName name="RangeReference" localSheetId="2">Sheet2!$B$2:$C$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -898,15 +899,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -924,6 +916,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1266,7 +1267,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:P203"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
@@ -1281,30 +1282,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="G1" s="110" t="s">
+      <c r="G1" s="107" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
-      <c r="M1" s="111"/>
-      <c r="N1" s="111"/>
-      <c r="O1" s="111"/>
-      <c r="P1" s="112"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="108"/>
+      <c r="L1" s="108"/>
+      <c r="M1" s="108"/>
+      <c r="N1" s="108"/>
+      <c r="O1" s="108"/>
+      <c r="P1" s="109"/>
     </row>
     <row r="2" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G2" s="113"/>
-      <c r="H2" s="114"/>
-      <c r="I2" s="114"/>
-      <c r="J2" s="114"/>
-      <c r="K2" s="114"/>
-      <c r="L2" s="114"/>
-      <c r="M2" s="114"/>
-      <c r="N2" s="114"/>
-      <c r="O2" s="114"/>
-      <c r="P2" s="115"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="111"/>
+      <c r="O2" s="111"/>
+      <c r="P2" s="112"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C3" s="64" t="s">
@@ -1317,11 +1318,11 @@
     <row r="4" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C4" s="65">
         <f ca="1">EDATE(D4,-12)</f>
-        <v>43693</v>
+        <v>43695</v>
       </c>
       <c r="D4" s="65">
         <f ca="1">TODAY()</f>
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="G4" t="str">
         <f t="array" aca="1" ref="G4:M203" ca="1">_xll.GetHistoricDataFromYahoo(C7,C4,D4)</f>
@@ -7353,10 +7354,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A2:P162"/>
+  <dimension ref="A2:T162"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="P113" sqref="P113"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="L112" sqref="L112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7401,7 +7402,7 @@
       </c>
       <c r="L3" s="9">
         <f t="array" aca="1" ref="L3:N5" ca="1">_xll.SystemTime()</f>
-        <v>206.46099509999999</v>
+        <v>52.781045599999999</v>
       </c>
       <c r="M3" s="10" t="str">
         <f ca="1"/>
@@ -7432,7 +7433,7 @@
       </c>
       <c r="M4" s="39">
         <f ca="1"/>
-        <v>3.7299999999999999E-5</v>
+        <v>8.3000000000000002E-6</v>
       </c>
       <c r="N4" s="14" t="e">
         <f ca="1"/>
@@ -8350,98 +8351,322 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>40</v>
       </c>
       <c r="B100" s="41"/>
     </row>
-    <row r="101" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>38</v>
       </c>
-      <c r="C102" s="68" t="str">
+      <c r="C102" s="68">
         <f ca="1">_xll.GetThreadId()</f>
-        <v>System.NotImplementedException : THREADSAFE NOT IMPLEMENTED IN netcore</v>
-      </c>
-      <c r="D102" s="69" t="str">
+        <v>5</v>
+      </c>
+      <c r="D102" s="69">
         <f ca="1">_xll.GetThreadId()</f>
-        <v>System.NotImplementedException : THREADSAFE NOT IMPLEMENTED IN netcore</v>
-      </c>
-      <c r="E102" s="69" t="str">
+        <v>10</v>
+      </c>
+      <c r="E102" s="69">
         <f ca="1">_xll.GetThreadId()</f>
-        <v>System.NotImplementedException : THREADSAFE NOT IMPLEMENTED IN netcore</v>
-      </c>
-      <c r="F102" s="70" t="str">
+        <v>7</v>
+      </c>
+      <c r="F102" s="70">
         <f ca="1">_xll.GetThreadId()</f>
-        <v>System.NotImplementedException : THREADSAFE NOT IMPLEMENTED IN netcore</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C103" s="71" t="str">
+        <v>5</v>
+      </c>
+      <c r="G102" s="70">
         <f ca="1">_xll.GetThreadId()</f>
-        <v>System.NotImplementedException : THREADSAFE NOT IMPLEMENTED IN netcore</v>
-      </c>
-      <c r="D103" s="72" t="str">
+        <v>7</v>
+      </c>
+      <c r="H102" s="70">
         <f ca="1">_xll.GetThreadId()</f>
-        <v>System.NotImplementedException : THREADSAFE NOT IMPLEMENTED IN netcore</v>
-      </c>
-      <c r="E103" s="72" t="str">
+        <v>9</v>
+      </c>
+      <c r="I102" s="70">
         <f ca="1">_xll.GetThreadId()</f>
-        <v>System.NotImplementedException : THREADSAFE NOT IMPLEMENTED IN netcore</v>
-      </c>
-      <c r="F103" s="73" t="str">
+        <v>10</v>
+      </c>
+      <c r="J102" s="70">
         <f ca="1">_xll.GetThreadId()</f>
-        <v>System.NotImplementedException : THREADSAFE NOT IMPLEMENTED IN netcore</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C104" s="71" t="str">
+        <v>1</v>
+      </c>
+      <c r="K102" s="70">
         <f ca="1">_xll.GetThreadId()</f>
-        <v>System.NotImplementedException : THREADSAFE NOT IMPLEMENTED IN netcore</v>
-      </c>
-      <c r="D104" s="72" t="str">
+        <v>4</v>
+      </c>
+      <c r="L102" s="70">
         <f ca="1">_xll.GetThreadId()</f>
-        <v>System.NotImplementedException : THREADSAFE NOT IMPLEMENTED IN netcore</v>
-      </c>
-      <c r="E104" s="72" t="str">
+        <v>5</v>
+      </c>
+      <c r="M102" s="70">
         <f ca="1">_xll.GetThreadId()</f>
-        <v>System.NotImplementedException : THREADSAFE NOT IMPLEMENTED IN netcore</v>
-      </c>
-      <c r="F104" s="73" t="str">
+        <v>6</v>
+      </c>
+      <c r="N102" s="70">
         <f ca="1">_xll.GetThreadId()</f>
-        <v>System.NotImplementedException : THREADSAFE NOT IMPLEMENTED IN netcore</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C105" s="74" t="str">
+        <v>8</v>
+      </c>
+      <c r="O102" s="70">
         <f ca="1">_xll.GetThreadId()</f>
-        <v>System.NotImplementedException : THREADSAFE NOT IMPLEMENTED IN netcore</v>
-      </c>
-      <c r="D105" s="75" t="str">
+        <v>7</v>
+      </c>
+      <c r="P102" s="70">
         <f ca="1">_xll.GetThreadId()</f>
-        <v>System.NotImplementedException : THREADSAFE NOT IMPLEMENTED IN netcore</v>
-      </c>
-      <c r="E105" s="75" t="str">
+        <v>9</v>
+      </c>
+      <c r="Q102" s="70">
         <f ca="1">_xll.GetThreadId()</f>
-        <v>System.NotImplementedException : THREADSAFE NOT IMPLEMENTED IN netcore</v>
-      </c>
-      <c r="F105" s="76" t="str">
+        <v>10</v>
+      </c>
+      <c r="R102" s="70">
         <f ca="1">_xll.GetThreadId()</f>
-        <v>System.NotImplementedException : THREADSAFE NOT IMPLEMENTED IN netcore</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C107" s="107" t="s">
+        <v>1</v>
+      </c>
+      <c r="S102" s="70">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>4</v>
+      </c>
+      <c r="T102" s="70">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C103" s="71">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>4</v>
+      </c>
+      <c r="D103" s="72">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>9</v>
+      </c>
+      <c r="E103" s="72">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>8</v>
+      </c>
+      <c r="F103" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>4</v>
+      </c>
+      <c r="G103" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>6</v>
+      </c>
+      <c r="H103" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>8</v>
+      </c>
+      <c r="I103" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>7</v>
+      </c>
+      <c r="J103" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>9</v>
+      </c>
+      <c r="K103" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>10</v>
+      </c>
+      <c r="L103" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>1</v>
+      </c>
+      <c r="M103" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>4</v>
+      </c>
+      <c r="N103" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>5</v>
+      </c>
+      <c r="O103" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>6</v>
+      </c>
+      <c r="P103" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>8</v>
+      </c>
+      <c r="Q103" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>7</v>
+      </c>
+      <c r="R103" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>9</v>
+      </c>
+      <c r="S103" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>10</v>
+      </c>
+      <c r="T103" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C104" s="71">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>9</v>
+      </c>
+      <c r="D104" s="72">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>7</v>
+      </c>
+      <c r="E104" s="72">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>9</v>
+      </c>
+      <c r="F104" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>10</v>
+      </c>
+      <c r="G104" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>4</v>
+      </c>
+      <c r="H104" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>5</v>
+      </c>
+      <c r="I104" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>6</v>
+      </c>
+      <c r="J104" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>8</v>
+      </c>
+      <c r="K104" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>7</v>
+      </c>
+      <c r="L104" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>9</v>
+      </c>
+      <c r="M104" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>10</v>
+      </c>
+      <c r="N104" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>1</v>
+      </c>
+      <c r="O104" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>4</v>
+      </c>
+      <c r="P104" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>5</v>
+      </c>
+      <c r="Q104" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>6</v>
+      </c>
+      <c r="R104" s="73">
+        <f t="array" aca="1" ref="R104" ca="1">_xll.GetThreadId()</f>
+        <v>10</v>
+      </c>
+      <c r="S104" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>8</v>
+      </c>
+      <c r="T104" s="73">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C105" s="74">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>1</v>
+      </c>
+      <c r="D105" s="75">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>8</v>
+      </c>
+      <c r="E105" s="75">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>6</v>
+      </c>
+      <c r="F105" s="76">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>1</v>
+      </c>
+      <c r="G105" s="76">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>9</v>
+      </c>
+      <c r="H105" s="76">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>10</v>
+      </c>
+      <c r="I105" s="76">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>1</v>
+      </c>
+      <c r="J105" s="76">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>4</v>
+      </c>
+      <c r="K105" s="76">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>5</v>
+      </c>
+      <c r="L105" s="76">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>6</v>
+      </c>
+      <c r="M105" s="76">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>8</v>
+      </c>
+      <c r="N105" s="76">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>7</v>
+      </c>
+      <c r="O105" s="76">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>9</v>
+      </c>
+      <c r="P105" s="76">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>10</v>
+      </c>
+      <c r="Q105" s="76">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>1</v>
+      </c>
+      <c r="R105" s="76">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>4</v>
+      </c>
+      <c r="S105" s="76">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>5</v>
+      </c>
+      <c r="T105" s="76">
+        <f ca="1">_xll.GetThreadId()</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C107" s="113" t="s">
         <v>45</v>
       </c>
-      <c r="D107" s="107"/>
+      <c r="D107" s="113"/>
       <c r="E107" t="s">
         <v>46</v>
       </c>
@@ -8449,7 +8674,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>44</v>
       </c>
@@ -8465,7 +8690,7 @@
         <v>System.Exception : XlfOper not implemented directly in xlwDotNet</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D109" s="106" t="s">
         <v>21</v>
       </c>
@@ -8478,7 +8703,7 @@
         <v>System.Exception : XlfOper not implemented directly in xlwDotNet</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D110" s="53" t="b">
         <v>1</v>
       </c>
@@ -8491,7 +8716,7 @@
         <v>System.Exception : XlfOper not implemented directly in xlwDotNet</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D111" s="54"/>
       <c r="E111" s="60" t="str">
         <f>_xll.typeString(D111)</f>
@@ -8502,7 +8727,7 @@
         <v>System.Exception : XlfOper not implemented directly in xlwDotNet</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E112" s="56" t="str">
         <f>_xll.typeString()</f>
         <v>System.Exception : XlfOper not implemented directly in xlwDotNet</v>
@@ -8543,10 +8768,10 @@
       </c>
     </row>
     <row r="115" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C115" s="108" t="s">
+      <c r="C115" s="114" t="s">
         <v>52</v>
       </c>
-      <c r="D115" s="108"/>
+      <c r="D115" s="114"/>
       <c r="E115" s="57" t="str">
         <f>_xll.typeString(Sheet2!RangeReference)</f>
         <v>System.Exception : XlfOper not implemented directly in xlwDotNet</v>
@@ -8557,24 +8782,24 @@
       </c>
     </row>
     <row r="120" spans="1:16" ht="18" x14ac:dyDescent="0.25">
-      <c r="A120" s="109" t="s">
+      <c r="A120" s="115" t="s">
         <v>58</v>
       </c>
-      <c r="B120" s="109"/>
-      <c r="C120" s="109"/>
-      <c r="D120" s="109"/>
-      <c r="E120" s="109"/>
-      <c r="F120" s="109"/>
-      <c r="G120" s="109"/>
-      <c r="H120" s="109"/>
-      <c r="I120" s="109"/>
-      <c r="J120" s="109"/>
-      <c r="K120" s="109"/>
-      <c r="L120" s="109"/>
-      <c r="M120" s="109"/>
-      <c r="N120" s="109"/>
-      <c r="O120" s="109"/>
-      <c r="P120" s="109"/>
+      <c r="B120" s="115"/>
+      <c r="C120" s="115"/>
+      <c r="D120" s="115"/>
+      <c r="E120" s="115"/>
+      <c r="F120" s="115"/>
+      <c r="G120" s="115"/>
+      <c r="H120" s="115"/>
+      <c r="I120" s="115"/>
+      <c r="J120" s="115"/>
+      <c r="K120" s="115"/>
+      <c r="L120" s="115"/>
+      <c r="M120" s="115"/>
+      <c r="N120" s="115"/>
+      <c r="O120" s="115"/>
+      <c r="P120" s="115"/>
     </row>
     <row r="121" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="122" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>